<commit_message>
extra orgs are added for log in as a client
</commit_message>
<xml_diff>
--- a/organization.xlsx
+++ b/organization.xlsx
@@ -145,10 +145,10 @@
     <t xml:space="preserve">Matt Medeiros</t>
   </si>
   <si>
+    <t xml:space="preserve">InActive</t>
+  </si>
+  <si>
     <t xml:space="preserve">610 Investments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InActive</t>
   </si>
   <si>
     <t xml:space="preserve">1000 Light Bulbs</t>
@@ -267,7 +267,7 @@
       <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.54"/>
@@ -534,18 +534,18 @@
         <v>40</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>40</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -567,7 +567,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>